<commit_message>
start of rev1.1 mods
</commit_message>
<xml_diff>
--- a/OBC Development Board/Fabrication Package/BOM/Bill of Materials-OBC Development Board(Build).xlsx
+++ b/OBC Development Board/Fabrication Package/BOM/Bill of Materials-OBC Development Board(Build).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\Calgary to Space\OBC_PCB_hardware\OBC Development Board\Fabrication Package\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACCFC8A2-62A0-459D-9CEB-8AFAB4F81571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{68FB8E60-4F16-4AF6-8C5A-548DC0892F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{188BA733-1076-4D84-81DA-0C5782496064}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{A419E911-6248-44E9-8AD9-3F6BF515CF51}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-OBC Developme" sheetId="1" r:id="rId1"/>
@@ -860,7 +860,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{361308FF-634D-4001-8330-4510F74781C7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B99338E-265B-45C1-8418-F1E96929E024}">
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
resolve errors and generate design files
</commit_message>
<xml_diff>
--- a/OBC Development Board/Fabrication Package/BOM/Bill of Materials-OBC Development Board(Build).xlsx
+++ b/OBC Development Board/Fabrication Package/BOM/Bill of Materials-OBC Development Board(Build).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\Calgary to Space\OBC_PCB_hardware\OBC Development Board\Fabrication Package\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68FB8E60-4F16-4AF6-8C5A-548DC0892F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{26697F15-FAD2-478D-9BFC-88AD85B0D5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{A419E911-6248-44E9-8AD9-3F6BF515CF51}"/>
+    <workbookView xWindow="32355" yWindow="18465" windowWidth="21600" windowHeight="11385" xr2:uid="{7240B0C2-2B67-4E8F-B379-F801C48576C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-OBC Developme" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="197">
   <si>
     <t>Designator</t>
   </si>
@@ -67,7 +68,7 @@
     <t/>
   </si>
   <si>
-    <t>C1, C3, C4, C5, C6, C7, C8, C9, C10, C14, C15, C16, C17, C18, C19, C22, C23, C24, C25, C26, C27, C28, C29, C30, C32, C43, C44, C46</t>
+    <t>C1, C3, C4, C5, C6, C7, C8, C9, C10, C14, C15, C16, C17, C18, C19, C22, C23, C24, C25, C26, C27, C28, C29, C30, C32, C51, C53</t>
   </si>
   <si>
     <t>0.1 µF ±10% 25V Ceramic Capacitor X7R 0603 (1608 Metric)</t>
@@ -85,7 +86,7 @@
     <t>CL10B104KA8NNNC</t>
   </si>
   <si>
-    <t>C2, C31, C39, C40, C45</t>
+    <t>C2, C31</t>
   </si>
   <si>
     <t>CAP CER 1UF 25V X7R 0603</t>
@@ -100,7 +101,7 @@
     <t>CC0603KRX7R8BB105</t>
   </si>
   <si>
-    <t>C11, C13</t>
+    <t>C11, C13, C48, C49, C50</t>
   </si>
   <si>
     <t>4.7 µF Molded Tantalum Capacitors 20 V 1206 (3216 Metric) 4Ohm</t>
@@ -115,7 +116,7 @@
     <t>TAJA475K020RNJ</t>
   </si>
   <si>
-    <t>C20</t>
+    <t>C12, C20</t>
   </si>
   <si>
     <t>CAP CER 0.1UF 25V X7R 0402</t>
@@ -142,16 +143,88 @@
     <t>CC0402FRNPO9BN150</t>
   </si>
   <si>
-    <t>C42</t>
-  </si>
-  <si>
-    <t>15 pF ±1% 50V Ceramic Capacitor C0G, NP0 0201 (0603 Metric)</t>
-  </si>
-  <si>
-    <t>1276-1048-1-ND</t>
-  </si>
-  <si>
-    <t>CL10C221JB8NNNC</t>
+    <t>C33</t>
+  </si>
+  <si>
+    <t>CAP TANT 22UF 10% 10V 1206</t>
+  </si>
+  <si>
+    <t>478-11193-1-ND</t>
+  </si>
+  <si>
+    <t>KYOCERA AVX</t>
+  </si>
+  <si>
+    <t>TPSA226K010T0900</t>
+  </si>
+  <si>
+    <t>C34, C35, C36</t>
+  </si>
+  <si>
+    <t>CAP ALUM POLY 47UF 20% 25V SMD</t>
+  </si>
+  <si>
+    <t>P16513CT-ND</t>
+  </si>
+  <si>
+    <t>Panasonic Electronic Components</t>
+  </si>
+  <si>
+    <t>25SVPF47M</t>
+  </si>
+  <si>
+    <t>C39, C44</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 16V X7R 0603</t>
+  </si>
+  <si>
+    <t>490-GRM188Z71C475KE21JCT-ND</t>
+  </si>
+  <si>
+    <t>Murata Electronics</t>
+  </si>
+  <si>
+    <t>GRM188Z71C475KE21J</t>
+  </si>
+  <si>
+    <t>C42, C45, C47</t>
+  </si>
+  <si>
+    <t>CAP CER 100PF 50V X7R 0603</t>
+  </si>
+  <si>
+    <t>311-3601-1-ND</t>
+  </si>
+  <si>
+    <t>CC0603KRX7R9BB101</t>
+  </si>
+  <si>
+    <t>C43, C46</t>
+  </si>
+  <si>
+    <t>CAP CER 33PF 50V X7R 0603</t>
+  </si>
+  <si>
+    <t>399-C0603C330K5RAC7867CT-ND</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>C0603C330K5RAC7867</t>
+  </si>
+  <si>
+    <t>C52</t>
+  </si>
+  <si>
+    <t>CAP CER 10000PF 50V X7R 0603</t>
+  </si>
+  <si>
+    <t>1276-1009-1-ND</t>
+  </si>
+  <si>
+    <t>CL10B103KB8NNNC</t>
   </si>
   <si>
     <t>D1, D2, D3, D4, D5, D6</t>
@@ -169,19 +242,22 @@
     <t>SML-D12U1WT86</t>
   </si>
   <si>
-    <t>J1, J2</t>
-  </si>
-  <si>
-    <t>CONN HEADER VERT 6POS 2.54MM</t>
-  </si>
-  <si>
-    <t>Samtec</t>
-  </si>
-  <si>
-    <t>TSW-106-05-T-S</t>
-  </si>
-  <si>
-    <t>J3</t>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 40V 5A SMC</t>
+  </si>
+  <si>
+    <t>B540C-FDICT-ND</t>
+  </si>
+  <si>
+    <t>Diodes Incorporated</t>
+  </si>
+  <si>
+    <t>B540C-13-F</t>
+  </si>
+  <si>
+    <t>J3, J8</t>
   </si>
   <si>
     <t>CONN HEADER SMD R/A 8POS 1.25MM</t>
@@ -193,6 +269,15 @@
     <t>WM7626CT-ND</t>
   </si>
   <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>CONN HEADER SMD R/A 4POS 1.25MM</t>
+  </si>
+  <si>
+    <t>WM7622CT-ND</t>
+  </si>
+  <si>
     <t>J5, J6</t>
   </si>
   <si>
@@ -208,7 +293,7 @@
     <t>ESQ-126-14-G-D</t>
   </si>
   <si>
-    <t>J7, J11</t>
+    <t>J7, J9, J11</t>
   </si>
   <si>
     <t>CONN HEADER SMD R/A 6POS 1.25MM</t>
@@ -217,7 +302,22 @@
     <t>WM7624CT-ND</t>
   </si>
   <si>
-    <t>J8, J12</t>
+    <t>J10, J13</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 10POS 1.25MM</t>
+  </si>
+  <si>
+    <t>WM1739-ND</t>
+  </si>
+  <si>
+    <t>Molex</t>
+  </si>
+  <si>
+    <t>0530471010</t>
+  </si>
+  <si>
+    <t>J12</t>
   </si>
   <si>
     <t>Connector Header Surface Mount, Right Angle 14 position 0.049 (1.25mm)</t>
@@ -226,25 +326,40 @@
     <t>900-0532617014CT-ND</t>
   </si>
   <si>
-    <t>Molex</t>
-  </si>
-  <si>
     <t>0532617014</t>
   </si>
   <si>
-    <t>J10, J13</t>
-  </si>
-  <si>
-    <t>CONN HEADER VERT 10POS 1.25MM</t>
-  </si>
-  <si>
-    <t>WM1739-ND</t>
-  </si>
-  <si>
-    <t>0530471010</t>
-  </si>
-  <si>
-    <t>R1, R2</t>
+    <t>J14, J16, J17, J18, J20</t>
+  </si>
+  <si>
+    <t>CONN MCX RCPT STR 50 OHM PCB</t>
+  </si>
+  <si>
+    <t>ACX1262-ND</t>
+  </si>
+  <si>
+    <t>Amphenol RF</t>
+  </si>
+  <si>
+    <t>252105</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>FIXED IND 6.8UH 8A 23.3 MOHM SMD</t>
+  </si>
+  <si>
+    <t>541-1303-1-ND</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
+    <t>IHLP4040DZER6R8M01</t>
+  </si>
+  <si>
+    <t>R1, R2, R3</t>
   </si>
   <si>
     <t>220 Ohms ±0.5% 0.063W, 1/16W Chip Resistor 0603 (1608 Metric) - Thin Film</t>
@@ -259,7 +374,7 @@
     <t>RR0816P-221-D</t>
   </si>
   <si>
-    <t>R4, R24, R27, R28, R30, R31, R32, R33, R34, R35, R36, R37, R38, R39, R41, R42, R43, R44, R45, R46, R47, R51, R52, R53, R55, R138</t>
+    <t>R4, R5, R6, R7, R13, R14, R15, R16, R17, R22, R24, R26, R27, R28, R30, R31, R32, R33, R34, R35, R36, R37, R38, R41, R42, R43, R44, R45, R46, R47, R51, R52, R53, R55, R63, R64, R67</t>
   </si>
   <si>
     <t>0 Ohms Jumper 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
@@ -274,7 +389,7 @@
     <t>RMCF0603ZT0R00</t>
   </si>
   <si>
-    <t>R8, R11, R13, R15, R16, R18, R21, R23</t>
+    <t>R8, R11</t>
   </si>
   <si>
     <t>RES SMD 1K OHM 1% 1/16W 0603</t>
@@ -289,7 +404,7 @@
     <t>CPF0603F1K0C1</t>
   </si>
   <si>
-    <t>R9, R10, R25, R29, R48, R50, R107</t>
+    <t>R9, R10, R12, R18, R21, R23, R25, R29, R39, R40, R48, R50, R56, R57, R58, R59, R107, R109</t>
   </si>
   <si>
     <t>22 Ohms ±0.5% 0.063W, 1/16W Chip Resistor 0603 (1608 Metric) - Thin Film</t>
@@ -301,7 +416,49 @@
     <t>RR0816Q-220-D</t>
   </si>
   <si>
-    <t>R14, R17, R130, R131, R146</t>
+    <t>R19, R20, R49, R54, R91, R92</t>
+  </si>
+  <si>
+    <t>RES SMD 4.7K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>CR0603-FX-4701ELFCT-ND</t>
+  </si>
+  <si>
+    <t>Bourns Inc.</t>
+  </si>
+  <si>
+    <t>CR0603-FX-4701ELF</t>
+  </si>
+  <si>
+    <t>R60, R61, R65, R66, R117, R118, R119, R120, R124, R125, R126, R127, R128, R129, R136</t>
+  </si>
+  <si>
+    <t>RES 10K OHM 1% 1/8W 0603, 10 kOhms ±0.1% 0.063W, 1/16W Chip Resistor 0603 (1608 Metric) - Thin Film</t>
+  </si>
+  <si>
+    <t>RNCP0603FTD10K0CT-ND, A119886CT-ND</t>
+  </si>
+  <si>
+    <t>Stackpole Electronics Inc, TE Connectivity Passive Product</t>
+  </si>
+  <si>
+    <t>RNCP0603FTD10K0, CPF0603B10KE</t>
+  </si>
+  <si>
+    <t>R62</t>
+  </si>
+  <si>
+    <t>RES 0.5 OHM 1% 1W 2010</t>
+  </si>
+  <si>
+    <t>541-10112-1-ND</t>
+  </si>
+  <si>
+    <t>WSLT2010R5000FEA18</t>
+  </si>
+  <si>
+    <t>R130, R131</t>
   </si>
   <si>
     <t>RES SMD 100 OHM 0.5% 1/16W 0603</t>
@@ -310,33 +467,6 @@
     <t>RR08P100DCT-ND</t>
   </si>
   <si>
-    <t>R49, R54</t>
-  </si>
-  <si>
-    <t>RES SMD 4.7K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>CR0603-FX-4701ELFCT-ND</t>
-  </si>
-  <si>
-    <t>Bourns Inc.</t>
-  </si>
-  <si>
-    <t>CR0603-FX-4701ELF</t>
-  </si>
-  <si>
-    <t>R117, R118, R119, R120, R121, R122, R123, R124, R125, R126, R127, R128, R129, R136, R140, R141</t>
-  </si>
-  <si>
-    <t>10 kOhms ±0.1% 0.063W, 1/16W Chip Resistor 0603 (1608 Metric) - Thin Film</t>
-  </si>
-  <si>
-    <t>A119886CT-ND</t>
-  </si>
-  <si>
-    <t>CPF0603B10KE</t>
-  </si>
-  <si>
     <t>R134, R135</t>
   </si>
   <si>
@@ -349,16 +479,10 @@
     <t>RC0402JR-07220RL</t>
   </si>
   <si>
-    <t>R142</t>
-  </si>
-  <si>
-    <t>RES 0.1 OHM 1% 3W 2512</t>
-  </si>
-  <si>
-    <t>CRA2512-FZ-R100ELFCT-ND</t>
-  </si>
-  <si>
-    <t>CRA2512-FZ-R100ELF</t>
+    <t>TP1, TP2</t>
+  </si>
+  <si>
+    <t>Test Point</t>
   </si>
   <si>
     <t>U1</t>
@@ -394,16 +518,16 @@
     <t>U4</t>
   </si>
   <si>
-    <t>IC DECODER/DEMUX 1X3:8 16TSSOP</t>
-  </si>
-  <si>
-    <t>74LCX138MTC-ND</t>
-  </si>
-  <si>
-    <t>onsemi</t>
-  </si>
-  <si>
-    <t>74LCX138MTC</t>
+    <t>IC REG BUCK ADJUSTABLE 3A 8SOIC</t>
+  </si>
+  <si>
+    <t>505-ADP2303ARDZ-ND</t>
+  </si>
+  <si>
+    <t>Analog Devices Inc.</t>
+  </si>
+  <si>
+    <t>ADP2303ARDZ</t>
   </si>
   <si>
     <t>U7, U8</t>
@@ -418,7 +542,7 @@
     <t>CY15B108QN-40LPXI</t>
   </si>
   <si>
-    <t>U9, U15</t>
+    <t>U9</t>
   </si>
   <si>
     <t>IC TRNSLTR BIDIRECTIONAL 14TSSOP</t>
@@ -448,43 +572,64 @@
     <t>MAX3086EESD+T</t>
   </si>
   <si>
+    <t>U11, U12</t>
+  </si>
+  <si>
+    <t>LORA-E5 WIRELESS MODULE (TAPE RE</t>
+  </si>
+  <si>
+    <t>1597-317990829CT-ND</t>
+  </si>
+  <si>
+    <t>Seeed Technology Co., Ltd</t>
+  </si>
+  <si>
+    <t>317990829</t>
+  </si>
+  <si>
+    <t>U13</t>
+  </si>
+  <si>
+    <t>IC RF SWITCH SPDT 3GHZ 6MLPD</t>
+  </si>
+  <si>
+    <t>Skyworks Solutions Inc.</t>
+  </si>
+  <si>
+    <t>SKY13323-378LF</t>
+  </si>
+  <si>
     <t>U14</t>
   </si>
   <si>
-    <t>IC MOTOR DRIVER 4.5V-36V 16TSSOP</t>
-  </si>
-  <si>
-    <t>MAX14871EUE+CT-ND</t>
-  </si>
-  <si>
-    <t>MAX14871EUE+T</t>
-  </si>
-  <si>
-    <t>U16</t>
-  </si>
-  <si>
-    <t>IC RECEIVER 0/4 16SO</t>
-  </si>
-  <si>
-    <t>MAX3095CSE+TCT-ND</t>
-  </si>
-  <si>
-    <t>MAX3095CSE+T</t>
+    <t>IC INVERT SCHMITT 1CH 1IN SC70</t>
   </si>
   <si>
     <t>Y1</t>
   </si>
   <si>
-    <t>XTAL OSC XO 25.0000MHZ HCMOS TTL</t>
-  </si>
-  <si>
-    <t>535-10819-1-ND</t>
-  </si>
-  <si>
-    <t>ABRACON</t>
-  </si>
-  <si>
-    <t>ASFL1-25.000MHZ-L-T</t>
+    <t>XTAL OSC TCXO 20.0000MHZ CSWV</t>
+  </si>
+  <si>
+    <t>114-TG2520SMN20.0000M-MCGNNM3CT-ND</t>
+  </si>
+  <si>
+    <t>EPSON</t>
+  </si>
+  <si>
+    <t>TG2520SMN 20.0000M-MCGNNM3</t>
+  </si>
+  <si>
+    <t>Y2</t>
+  </si>
+  <si>
+    <t>XTAL OSC TCXO 32.7680KHZ CMOS</t>
+  </si>
+  <si>
+    <t>SER4422CT-ND</t>
+  </si>
+  <si>
+    <t>TG-3541CE 32.7680KXB3</t>
   </si>
 </sst>
 </file>
@@ -860,8 +1005,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B99338E-265B-45C1-8418-F1E96929E024}">
-  <dimension ref="A1:G33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95155635-C2A1-467D-84E4-29A919324E7B}">
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -917,7 +1062,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
@@ -940,7 +1085,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>11</v>
@@ -963,7 +1108,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>11</v>
@@ -986,7 +1131,7 @@
         <v>26</v>
       </c>
       <c r="C6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
@@ -1041,79 +1186,87 @@
         <v>36</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="D10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="F10" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
@@ -1122,171 +1275,163 @@
         <v>11</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C14" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C16" s="1">
         <v>2</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>72</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="1">
-        <v>26</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="E17" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>77</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C18" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C19" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G19" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -1296,7 +1441,7 @@
         <v>88</v>
       </c>
       <c r="C20" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>11</v>
@@ -1305,223 +1450,225 @@
         <v>89</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C21" s="1">
-        <v>2</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="G21" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C22" s="1">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C23" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>18</v>
+        <v>104</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C24" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C25" s="1">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E25" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="F25" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C26" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C27" s="1">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C28" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C29" s="1">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
@@ -1530,82 +1677,317 @@
         <v>11</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C31" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C32" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>129</v>
+        <v>18</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C33" s="1">
+        <v>2</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C34" s="1">
         <v>1</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>148</v>
+      <c r="D34" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C35" s="1">
+        <v>4</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C37" s="1">
+        <v>2</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C40" s="1">
+        <v>2</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C42" s="1">
+        <v>1</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>